<commit_message>
More updates on the survey analysis
</commit_message>
<xml_diff>
--- a/results/survey_analysis.xlsx
+++ b/results/survey_analysis.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fronchettl\Documents\GitHub\USP-2020\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DECFDF-2A3F-4572-B66E-779B002CB747}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A684AC7B-AD3B-457B-972D-29B7D1615A78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8513" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Demographics" sheetId="3" r:id="rId2"/>
-    <sheet name="Comments" sheetId="2" r:id="rId3"/>
+    <sheet name="Categories" sheetId="4" r:id="rId2"/>
+    <sheet name="Demographics" sheetId="3" r:id="rId3"/>
+    <sheet name="Comments" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="121">
   <si>
     <t>Progress</t>
   </si>
@@ -343,6 +344,48 @@
   </si>
   <si>
     <t>Removed participants who got more than one question wrong.</t>
+  </si>
+  <si>
+    <t>Previous Programming Experience</t>
+  </si>
+  <si>
+    <t>Non-Coder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Experience in OSS</t>
+  </si>
+  <si>
+    <t>OSS Participation Type</t>
+  </si>
+  <si>
+    <t>Contributed to documentation?</t>
+  </si>
+  <si>
+    <t>Choose a task</t>
+  </si>
+  <si>
+    <t>Talk to the community</t>
+  </si>
+  <si>
+    <t>Build local workspace</t>
+  </si>
+  <si>
+    <t>Contribution flow</t>
+  </si>
+  <si>
+    <t>Deal with the code</t>
+  </si>
+  <si>
+    <t>Submit the changes</t>
+  </si>
+  <si>
+    <t>Total evaluations:</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -373,7 +416,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +488,60 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE95959"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBEB7FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -458,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -481,9 +578,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -494,531 +588,38 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1093,14 +694,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBEB7FF"/>
+      <color rgb="FFE95959"/>
+      <color rgb="FFB7FFDB"/>
+      <color rgb="FFEDB9FF"/>
+      <color rgb="FFB3CB77"/>
+      <color rgb="FF43FFC0"/>
+      <color rgb="FFE497FF"/>
+      <color rgb="FF66CCFF"/>
       <color rgb="FFFFA3E0"/>
       <color rgb="FFFFA365"/>
-      <color rgb="FFC86400"/>
-      <color rgb="FFCCB3FF"/>
-      <color rgb="FFFF8F75"/>
-      <color rgb="FFFFB481"/>
-      <color rgb="FF93DBFF"/>
-      <color rgb="FF66CCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1112,6 +715,1725 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Programming Experience</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Demographics!$B$3:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No experience</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Less than or equal to 3 years</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Greater than 3 years and less than 15 years</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Greater than or equal to 15 years</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Demographics!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EAFF-4E59-8FB5-F894468BE059}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="245847535"/>
+        <c:axId val="247352351"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="245847535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="247352351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="247352351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="245847535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200" b="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="104"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="4"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Experience in OSS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Demographics!$B$9:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No experience</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Less than or equal to 3 years</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Greater than 3 years and less than 15 years</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Greater than or equal to 15 years</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Demographics!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-61E1-4F2F-93F4-37079A8DBF4B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="248159023"/>
+        <c:axId val="558470063"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="248159023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="558470063"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="558470063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="248159023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
+  <a:schemeClr val="accent2"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA0E7F49-8665-444E-BAF7-A73E41EA3644}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F75BD643-5AEE-4CA1-A491-B13626065202}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1413,9 +2735,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+    <sheetView topLeftCell="AV1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AY4" sqref="AY4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1433,35 +2755,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:75" x14ac:dyDescent="0.45">
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="AY1" s="18" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="AY1" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:75" ht="62.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>89</v>
       </c>
       <c r="AY2" s="1" t="s">
@@ -1619,7 +2941,7 @@
       <c r="AX4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AY4" s="17" t="s">
+      <c r="AY4" s="16" t="s">
         <v>49</v>
       </c>
       <c r="AZ4" s="11" t="s">
@@ -1696,7 +3018,7 @@
       </c>
     </row>
     <row r="5" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <v>100</v>
       </c>
       <c r="B5" s="4">
@@ -1923,7 +3245,7 @@
       </c>
     </row>
     <row r="6" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>100</v>
       </c>
       <c r="B6" s="4">
@@ -2150,7 +3472,7 @@
       </c>
     </row>
     <row r="7" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>100</v>
       </c>
       <c r="B7" s="4">
@@ -2377,7 +3699,7 @@
       </c>
     </row>
     <row r="8" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <v>100</v>
       </c>
       <c r="B8" s="4">
@@ -2604,7 +3926,7 @@
       </c>
     </row>
     <row r="9" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>100</v>
       </c>
       <c r="B9" s="4">
@@ -2831,7 +4153,7 @@
       </c>
     </row>
     <row r="10" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>100</v>
       </c>
       <c r="B10" s="4">
@@ -3058,7 +4380,7 @@
       </c>
     </row>
     <row r="11" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>100</v>
       </c>
       <c r="B11" s="4">
@@ -3285,7 +4607,7 @@
       </c>
     </row>
     <row r="12" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>100</v>
       </c>
       <c r="B12" s="4">
@@ -3512,7 +4834,7 @@
       </c>
     </row>
     <row r="13" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A13" s="16">
+      <c r="A13" s="15">
         <v>100</v>
       </c>
       <c r="B13" s="4">
@@ -3739,7 +5061,7 @@
       </c>
     </row>
     <row r="14" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <v>100</v>
       </c>
       <c r="B14" s="4">
@@ -3966,7 +5288,7 @@
       </c>
     </row>
     <row r="15" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A15" s="16">
+      <c r="A15" s="15">
         <v>100</v>
       </c>
       <c r="B15" s="4">
@@ -4193,7 +5515,7 @@
       </c>
     </row>
     <row r="16" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>100</v>
       </c>
       <c r="B16" s="4">
@@ -4420,7 +5742,7 @@
       </c>
     </row>
     <row r="17" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>100</v>
       </c>
       <c r="B17" s="4">
@@ -4647,7 +5969,7 @@
       </c>
     </row>
     <row r="18" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A18" s="16">
+      <c r="A18" s="15">
         <v>100</v>
       </c>
       <c r="B18" s="4">
@@ -4874,7 +6196,7 @@
       </c>
     </row>
     <row r="19" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A19" s="16">
+      <c r="A19" s="15">
         <v>100</v>
       </c>
       <c r="B19" s="4">
@@ -5101,7 +6423,7 @@
       </c>
     </row>
     <row r="20" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A20" s="16">
+      <c r="A20" s="15">
         <v>100</v>
       </c>
       <c r="B20" s="4">
@@ -5328,7 +6650,7 @@
       </c>
     </row>
     <row r="21" spans="1:75" ht="327.75" x14ac:dyDescent="0.45">
-      <c r="A21" s="16">
+      <c r="A21" s="15">
         <v>100</v>
       </c>
       <c r="B21" s="4">
@@ -5602,18 +6924,632 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984236D5-FEDA-41FB-BF72-A4D6E541FB35}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E493030-D07F-4844-B15C-53B8AC396BAD}">
+  <dimension ref="B2:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="30.59765625" customWidth="1"/>
+    <col min="3" max="4" width="12.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B2" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3">
+        <f>COUNTIF(Data!J5:S21,B3)</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="25">
+        <f>C3/C$7*100</f>
+        <v>15.686274509803921</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4">
+        <f>COUNTIF(Data!J5:S21,B4)</f>
+        <v>8</v>
+      </c>
+      <c r="D4" s="25">
+        <f t="shared" ref="D4:D6" si="0">C4/C$7*100</f>
+        <v>15.686274509803921</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <f>COUNTIF(Data!J5:S21,B5)</f>
+        <v>19</v>
+      </c>
+      <c r="D5" s="25">
+        <f t="shared" si="0"/>
+        <v>37.254901960784316</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6">
+        <f>COUNTIF(Data!J5:S21,B6)</f>
+        <v>16</v>
+      </c>
+      <c r="D6" s="25">
+        <f t="shared" si="0"/>
+        <v>31.372549019607842</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C3:C6)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="19"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10">
+        <f>COUNTIF(Data!T5:AC21,B10)</f>
+        <v>4</v>
+      </c>
+      <c r="D10" s="25">
+        <f>C10/C$14*100</f>
+        <v>7.8431372549019605</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11">
+        <f>COUNTIF(Data!T5:AC21,B11)</f>
+        <v>11</v>
+      </c>
+      <c r="D11" s="25">
+        <f t="shared" ref="D11:D13" si="1">C11/C$14*100</f>
+        <v>21.568627450980394</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12">
+        <f>COUNTIF(Data!T5:AC21,B12)</f>
+        <v>18</v>
+      </c>
+      <c r="D12" s="25">
+        <f t="shared" si="1"/>
+        <v>35.294117647058826</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13">
+        <f>COUNTIF(Data!T5:AC21,B13)</f>
+        <v>18</v>
+      </c>
+      <c r="D13" s="25">
+        <f t="shared" si="1"/>
+        <v>35.294117647058826</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C10:C13)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B15" s="19"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B16" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17">
+        <f>COUNTIF(Data!AD5:AM21,B17)</f>
+        <v>4</v>
+      </c>
+      <c r="D17" s="25">
+        <f>C17/C$21*100</f>
+        <v>7.8431372549019605</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18">
+        <f>COUNTIF(Data!AD5:AM21,B18)</f>
+        <v>11</v>
+      </c>
+      <c r="D18" s="25">
+        <f t="shared" ref="D18:D20" si="2">C18/C$21*100</f>
+        <v>21.568627450980394</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19">
+        <f>COUNTIF(Data!AD5:AM21,B19)</f>
+        <v>19</v>
+      </c>
+      <c r="D19" s="25">
+        <f t="shared" si="2"/>
+        <v>37.254901960784316</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20">
+        <f>COUNTIF(Data!AD5:AM21,B20)</f>
+        <v>17</v>
+      </c>
+      <c r="D20" s="25">
+        <f t="shared" si="2"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B21" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21">
+        <f>SUM(C17:C20)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B22" s="19"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24">
+        <f>COUNTIF(Data!AN5:AW21,B24)</f>
+        <v>4</v>
+      </c>
+      <c r="D24" s="25">
+        <f>C24/C$28*100</f>
+        <v>7.8431372549019605</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25">
+        <f>COUNTIF(Data!AN5:AW21,B25)</f>
+        <v>8</v>
+      </c>
+      <c r="D25" s="25">
+        <f t="shared" ref="D25:D27" si="3">C25/C$28*100</f>
+        <v>15.686274509803921</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <f>COUNTIF(Data!AN5:AW21,B26)</f>
+        <v>15</v>
+      </c>
+      <c r="D26" s="25">
+        <f t="shared" si="3"/>
+        <v>29.411764705882355</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27">
+        <f>COUNTIF(Data!AN5:AW21,B27)</f>
+        <v>24</v>
+      </c>
+      <c r="D27" s="25">
+        <f t="shared" si="3"/>
+        <v>47.058823529411761</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28">
+        <f>SUM(C24:C27)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B29" s="19"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B30" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31">
+        <f>COUNTIF(Data!AX5:BH21,B31)</f>
+        <v>3</v>
+      </c>
+      <c r="D31" s="25">
+        <f>C31/C$35*100</f>
+        <v>5.8823529411764701</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="24">
+        <f>COUNTIF(Data!AX5:BH21,B32) - 17</f>
+        <v>6</v>
+      </c>
+      <c r="D32" s="25">
+        <f t="shared" ref="D32:D34" si="4">C32/C$35*100</f>
+        <v>11.76470588235294</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33">
+        <f>COUNTIF(Data!AX5:BH21,B33)</f>
+        <v>22</v>
+      </c>
+      <c r="D33" s="25">
+        <f t="shared" si="4"/>
+        <v>43.137254901960787</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34">
+        <f>COUNTIF(Data!AX5:BH21,B34)</f>
+        <v>20</v>
+      </c>
+      <c r="D34" s="25">
+        <f t="shared" si="4"/>
+        <v>39.215686274509807</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B35" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35">
+        <f>SUM(C31:C34)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B36" s="19"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B37" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38">
+        <f>COUNTIF(Data!BI5:BR21,B38)</f>
+        <v>4</v>
+      </c>
+      <c r="D38" s="25">
+        <f>C38/C$42*100</f>
+        <v>7.8431372549019605</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39">
+        <f>COUNTIF(Data!BI5:BR21,B39)</f>
+        <v>10</v>
+      </c>
+      <c r="D39" s="25">
+        <f t="shared" ref="D39:D41" si="5">C39/C$42*100</f>
+        <v>19.607843137254903</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40">
+        <f>COUNTIF(Data!BI5:BR21,B40)</f>
+        <v>19</v>
+      </c>
+      <c r="D40" s="25">
+        <f t="shared" si="5"/>
+        <v>37.254901960784316</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41">
+        <f>COUNTIF(Data!BI5:BR21,B41)</f>
+        <v>18</v>
+      </c>
+      <c r="D41" s="25">
+        <f t="shared" si="5"/>
+        <v>35.294117647058826</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B42" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42">
+        <f>SUM(C38:C41)</f>
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984236D5-FEDA-41FB-BF72-A4D6E541FB35}">
+  <dimension ref="B2:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="33.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B2" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="20">
+        <f>COUNTIF(Data!BS5:BS21,B3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="20">
+        <f>COUNTIF(Data!BS5:BS21,B4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="20">
+        <f>COUNTIF(Data!BS5:BS21,B5)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="20">
+        <f>COUNTIF(Data!BS5:BS21,B6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B8" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9">
+        <f>COUNTIF(Data!BT5:BT21,B9)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10">
+        <f>COUNTIF(Data!BT6:BT22,B10)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <f>COUNTIF(Data!BT7:BT23,B11)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12">
+        <f>COUNTIF(Data!BT8:BT24,B12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B14" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15">
+        <f>COUNTIF(Data!BU5:BU21,Demographics!B15)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16">
+        <f>COUNTIF(Data!BU5:BU21,Demographics!B16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B18" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="23"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19">
+        <f>COUNTIF(Data!BV5:BV21,B19)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20">
+        <f>COUNTIF(Data!BV5:BV21,B20)</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B18:C18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25A1F8F-B585-4477-B738-9EFA58F05705}">
   <dimension ref="A2:A3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Mores updates in the survey analysis
</commit_message>
<xml_diff>
--- a/results/survey_analysis.xlsx
+++ b/results/survey_analysis.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fronchettl\Documents\GitHub\USP-2020\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A684AC7B-AD3B-457B-972D-29B7D1615A78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F2B54F-22FB-4CAE-9167-1C4E71344CCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8513" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8513" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Categories" sheetId="4" r:id="rId2"/>
-    <sheet name="Demographics" sheetId="3" r:id="rId3"/>
+    <sheet name="Demographics" sheetId="3" r:id="rId2"/>
+    <sheet name="Categories" sheetId="4" r:id="rId3"/>
     <sheet name="Comments" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="121">
   <si>
     <t>Progress</t>
   </si>
@@ -588,20 +588,8 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -613,6 +601,18 @@
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -694,6 +694,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF2121"/>
       <color rgb="FFBEB7FF"/>
       <color rgb="FFE95959"/>
       <color rgb="FFB7FFDB"/>
@@ -703,7 +704,6 @@
       <color rgb="FFE497FF"/>
       <color rgb="FF66CCFF"/>
       <color rgb="FFFFA3E0"/>
-      <color rgb="FFFFA365"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1310,6 +1310,698 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Categories Evaluation (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Categories!$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Extremely adequate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Categories!$I$4:$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Contribution flow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Choose a task</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Talk to the community</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Build local workspace</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Deal with the code</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Submit the changes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Categories!$I$5:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>31.372549019607842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.058823529411761</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.215686274509807</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.294117647058826</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6963-46E9-8E57-F9F901E57249}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Categories!$H$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Somewhat adequate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Categories!$I$4:$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Contribution flow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Choose a task</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Talk to the community</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Build local workspace</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Deal with the code</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Submit the changes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Categories!$I$6:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>37.254901960784316</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.254901960784316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.411764705882355</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.137254901960787</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.254901960784316</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6963-46E9-8E57-F9F901E57249}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Categories!$H$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Somewhat inadequate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Categories!$I$4:$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Contribution flow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Choose a task</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Talk to the community</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Build local workspace</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Deal with the code</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Submit the changes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Categories!$I$7:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15.686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.568627450980394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.568627450980394</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.76470588235294</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.607843137254903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6963-46E9-8E57-F9F901E57249}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Categories!$H$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Extremely inadequate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF2121"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Categories!$I$4:$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Contribution flow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Choose a task</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Talk to the community</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Build local workspace</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Deal with the code</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Submit the changes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Categories!$I$8:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15.686274509803921</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8431372549019605</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8431372549019605</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8431372549019605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8823529411764701</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8431372549019605</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6963-46E9-8E57-F9F901E57249}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="334517200"/>
+        <c:axId val="376753840"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="334517200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Categories</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="376753840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="376753840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334517200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
@@ -1350,6 +2042,43 @@
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
   <a:schemeClr val="accent2"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -2359,6 +3088,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2428,6 +3662,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1276350</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC70C89-6E82-4E58-91A1-CB48BC25316B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2735,9 +4010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW21"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AY4" sqref="AY4"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2755,14 +4030,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:75" x14ac:dyDescent="0.45">
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
       <c r="AY1" s="17" t="s">
         <v>104</v>
       </c>
@@ -6924,478 +8199,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E493030-D07F-4844-B15C-53B8AC396BAD}">
-  <dimension ref="B2:D42"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="30.59765625" customWidth="1"/>
-    <col min="3" max="4" width="12.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B2" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3">
-        <f>COUNTIF(Data!J5:S21,B3)</f>
-        <v>8</v>
-      </c>
-      <c r="D3" s="25">
-        <f>C3/C$7*100</f>
-        <v>15.686274509803921</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4">
-        <f>COUNTIF(Data!J5:S21,B4)</f>
-        <v>8</v>
-      </c>
-      <c r="D4" s="25">
-        <f t="shared" ref="D4:D6" si="0">C4/C$7*100</f>
-        <v>15.686274509803921</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5">
-        <f>COUNTIF(Data!J5:S21,B5)</f>
-        <v>19</v>
-      </c>
-      <c r="D5" s="25">
-        <f t="shared" si="0"/>
-        <v>37.254901960784316</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6">
-        <f>COUNTIF(Data!J5:S21,B6)</f>
-        <v>16</v>
-      </c>
-      <c r="D6" s="25">
-        <f t="shared" si="0"/>
-        <v>31.372549019607842</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B7" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7">
-        <f>SUM(C3:C6)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B8" s="19"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B9" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10">
-        <f>COUNTIF(Data!T5:AC21,B10)</f>
-        <v>4</v>
-      </c>
-      <c r="D10" s="25">
-        <f>C10/C$14*100</f>
-        <v>7.8431372549019605</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11">
-        <f>COUNTIF(Data!T5:AC21,B11)</f>
-        <v>11</v>
-      </c>
-      <c r="D11" s="25">
-        <f t="shared" ref="D11:D13" si="1">C11/C$14*100</f>
-        <v>21.568627450980394</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12">
-        <f>COUNTIF(Data!T5:AC21,B12)</f>
-        <v>18</v>
-      </c>
-      <c r="D12" s="25">
-        <f t="shared" si="1"/>
-        <v>35.294117647058826</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13">
-        <f>COUNTIF(Data!T5:AC21,B13)</f>
-        <v>18</v>
-      </c>
-      <c r="D13" s="25">
-        <f t="shared" si="1"/>
-        <v>35.294117647058826</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B14" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14">
-        <f>SUM(C10:C13)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B15" s="19"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B16" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17">
-        <f>COUNTIF(Data!AD5:AM21,B17)</f>
-        <v>4</v>
-      </c>
-      <c r="D17" s="25">
-        <f>C17/C$21*100</f>
-        <v>7.8431372549019605</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18">
-        <f>COUNTIF(Data!AD5:AM21,B18)</f>
-        <v>11</v>
-      </c>
-      <c r="D18" s="25">
-        <f t="shared" ref="D18:D20" si="2">C18/C$21*100</f>
-        <v>21.568627450980394</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19">
-        <f>COUNTIF(Data!AD5:AM21,B19)</f>
-        <v>19</v>
-      </c>
-      <c r="D19" s="25">
-        <f t="shared" si="2"/>
-        <v>37.254901960784316</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20">
-        <f>COUNTIF(Data!AD5:AM21,B20)</f>
-        <v>17</v>
-      </c>
-      <c r="D20" s="25">
-        <f t="shared" si="2"/>
-        <v>33.333333333333329</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B21" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21">
-        <f>SUM(C17:C20)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B22" s="19"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B23" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24">
-        <f>COUNTIF(Data!AN5:AW21,B24)</f>
-        <v>4</v>
-      </c>
-      <c r="D24" s="25">
-        <f>C24/C$28*100</f>
-        <v>7.8431372549019605</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25">
-        <f>COUNTIF(Data!AN5:AW21,B25)</f>
-        <v>8</v>
-      </c>
-      <c r="D25" s="25">
-        <f t="shared" ref="D25:D27" si="3">C25/C$28*100</f>
-        <v>15.686274509803921</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26">
-        <f>COUNTIF(Data!AN5:AW21,B26)</f>
-        <v>15</v>
-      </c>
-      <c r="D26" s="25">
-        <f t="shared" si="3"/>
-        <v>29.411764705882355</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27">
-        <f>COUNTIF(Data!AN5:AW21,B27)</f>
-        <v>24</v>
-      </c>
-      <c r="D27" s="25">
-        <f t="shared" si="3"/>
-        <v>47.058823529411761</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B28" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28">
-        <f>SUM(C24:C27)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B29" s="19"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B30" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31">
-        <f>COUNTIF(Data!AX5:BH21,B31)</f>
-        <v>3</v>
-      </c>
-      <c r="D31" s="25">
-        <f>C31/C$35*100</f>
-        <v>5.8823529411764701</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="24">
-        <f>COUNTIF(Data!AX5:BH21,B32) - 17</f>
-        <v>6</v>
-      </c>
-      <c r="D32" s="25">
-        <f t="shared" ref="D32:D34" si="4">C32/C$35*100</f>
-        <v>11.76470588235294</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33">
-        <f>COUNTIF(Data!AX5:BH21,B33)</f>
-        <v>22</v>
-      </c>
-      <c r="D33" s="25">
-        <f t="shared" si="4"/>
-        <v>43.137254901960787</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34">
-        <f>COUNTIF(Data!AX5:BH21,B34)</f>
-        <v>20</v>
-      </c>
-      <c r="D34" s="25">
-        <f t="shared" si="4"/>
-        <v>39.215686274509807</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B35" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35">
-        <f>SUM(C31:C34)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B36" s="19"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B37" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="C37" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D37" s="32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38">
-        <f>COUNTIF(Data!BI5:BR21,B38)</f>
-        <v>4</v>
-      </c>
-      <c r="D38" s="25">
-        <f>C38/C$42*100</f>
-        <v>7.8431372549019605</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39">
-        <f>COUNTIF(Data!BI5:BR21,B39)</f>
-        <v>10</v>
-      </c>
-      <c r="D39" s="25">
-        <f t="shared" ref="D39:D41" si="5">C39/C$42*100</f>
-        <v>19.607843137254903</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40">
-        <f>COUNTIF(Data!BI5:BR21,B40)</f>
-        <v>19</v>
-      </c>
-      <c r="D40" s="25">
-        <f t="shared" si="5"/>
-        <v>37.254901960784316</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41">
-        <f>COUNTIF(Data!BI5:BR21,B41)</f>
-        <v>18</v>
-      </c>
-      <c r="D41" s="25">
-        <f t="shared" si="5"/>
-        <v>35.294117647058826</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B42" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42">
-        <f>SUM(C38:C41)</f>
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984236D5-FEDA-41FB-BF72-A4D6E541FB35}">
   <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7405,16 +8213,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <f>COUNTIF(Data!BS5:BS21,B3)</f>
         <v>0</v>
       </c>
@@ -7423,7 +8231,7 @@
       <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <f>COUNTIF(Data!BS5:BS21,B4)</f>
         <v>4</v>
       </c>
@@ -7432,7 +8240,7 @@
       <c r="B5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <f>COUNTIF(Data!BS5:BS21,B5)</f>
         <v>11</v>
       </c>
@@ -7441,16 +8249,16 @@
       <c r="B6" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <f>COUNTIF(Data!BS5:BS21,B6)</f>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="30"/>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
@@ -7489,10 +8297,10 @@
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
@@ -7513,10 +8321,10 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="32"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
@@ -7543,6 +8351,603 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B18:C18"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E493030-D07F-4844-B15C-53B8AC396BAD}">
+  <dimension ref="B2:N42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="30.59765625" customWidth="1"/>
+    <col min="3" max="4" width="12.59765625" customWidth="1"/>
+    <col min="8" max="8" width="21.86328125" customWidth="1"/>
+    <col min="9" max="14" width="20.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B2" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3">
+        <f>COUNTIF(Data!J5:S21,B3)</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="21">
+        <f>C3/C$7*100</f>
+        <v>15.686274509803921</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4">
+        <f>COUNTIF(Data!J5:S21,B4)</f>
+        <v>8</v>
+      </c>
+      <c r="D4" s="21">
+        <f t="shared" ref="D4:D6" si="0">C4/C$7*100</f>
+        <v>15.686274509803921</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <f>COUNTIF(Data!J5:S21,B5)</f>
+        <v>19</v>
+      </c>
+      <c r="D5" s="21">
+        <f t="shared" si="0"/>
+        <v>37.254901960784316</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="21">
+        <v>31.372549019607842</v>
+      </c>
+      <c r="J5" s="21">
+        <v>35.294117647058826</v>
+      </c>
+      <c r="K5" s="21">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="L5" s="21">
+        <v>47.058823529411761</v>
+      </c>
+      <c r="M5" s="21">
+        <v>39.215686274509807</v>
+      </c>
+      <c r="N5" s="21">
+        <v>35.294117647058826</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6">
+        <f>COUNTIF(Data!J5:S21,B6)</f>
+        <v>16</v>
+      </c>
+      <c r="D6" s="21">
+        <f t="shared" si="0"/>
+        <v>31.372549019607842</v>
+      </c>
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="21">
+        <v>37.254901960784316</v>
+      </c>
+      <c r="J6" s="21">
+        <v>35.294117647058826</v>
+      </c>
+      <c r="K6" s="21">
+        <v>37.254901960784316</v>
+      </c>
+      <c r="L6" s="21">
+        <v>29.411764705882355</v>
+      </c>
+      <c r="M6" s="21">
+        <v>43.137254901960787</v>
+      </c>
+      <c r="N6" s="21">
+        <v>37.254901960784316</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B7" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C3:C6)</f>
+        <v>51</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="H7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="21">
+        <v>15.686274509803921</v>
+      </c>
+      <c r="J7" s="21">
+        <v>21.568627450980394</v>
+      </c>
+      <c r="K7" s="21">
+        <v>21.568627450980394</v>
+      </c>
+      <c r="L7" s="21">
+        <v>15.686274509803921</v>
+      </c>
+      <c r="M7" s="21">
+        <v>11.76470588235294</v>
+      </c>
+      <c r="N7" s="21">
+        <v>19.607843137254903</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B8" s="18"/>
+      <c r="H8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="21">
+        <v>15.686274509803921</v>
+      </c>
+      <c r="J8" s="21">
+        <v>7.8431372549019605</v>
+      </c>
+      <c r="K8" s="21">
+        <v>7.8431372549019605</v>
+      </c>
+      <c r="L8" s="21">
+        <v>7.8431372549019605</v>
+      </c>
+      <c r="M8" s="21">
+        <v>5.8823529411764701</v>
+      </c>
+      <c r="N8" s="21">
+        <v>7.8431372549019605</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B9" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10">
+        <f>COUNTIF(Data!T5:AC21,B10)</f>
+        <v>4</v>
+      </c>
+      <c r="D10" s="21">
+        <f>C10/C$14*100</f>
+        <v>7.8431372549019605</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11">
+        <f>COUNTIF(Data!T5:AC21,B11)</f>
+        <v>11</v>
+      </c>
+      <c r="D11" s="21">
+        <f t="shared" ref="D11:D13" si="1">C11/C$14*100</f>
+        <v>21.568627450980394</v>
+      </c>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12">
+        <f>COUNTIF(Data!T5:AC21,B12)</f>
+        <v>18</v>
+      </c>
+      <c r="D12" s="21">
+        <f t="shared" si="1"/>
+        <v>35.294117647058826</v>
+      </c>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13">
+        <f>COUNTIF(Data!T5:AC21,B13)</f>
+        <v>18</v>
+      </c>
+      <c r="D13" s="21">
+        <f t="shared" si="1"/>
+        <v>35.294117647058826</v>
+      </c>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B14" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C10:C13)</f>
+        <v>51</v>
+      </c>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B15" s="18"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B16" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17">
+        <f>COUNTIF(Data!AD5:AM21,B17)</f>
+        <v>4</v>
+      </c>
+      <c r="D17" s="21">
+        <f>C17/C$21*100</f>
+        <v>7.8431372549019605</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18">
+        <f>COUNTIF(Data!AD5:AM21,B18)</f>
+        <v>11</v>
+      </c>
+      <c r="D18" s="21">
+        <f t="shared" ref="D18:D20" si="2">C18/C$21*100</f>
+        <v>21.568627450980394</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19">
+        <f>COUNTIF(Data!AD5:AM21,B19)</f>
+        <v>19</v>
+      </c>
+      <c r="D19" s="21">
+        <f t="shared" si="2"/>
+        <v>37.254901960784316</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20">
+        <f>COUNTIF(Data!AD5:AM21,B20)</f>
+        <v>17</v>
+      </c>
+      <c r="D20" s="21">
+        <f t="shared" si="2"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B21" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21">
+        <f>SUM(C17:C20)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B22" s="18"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24">
+        <f>COUNTIF(Data!AN5:AW21,B24)</f>
+        <v>4</v>
+      </c>
+      <c r="D24" s="21">
+        <f>C24/C$28*100</f>
+        <v>7.8431372549019605</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25">
+        <f>COUNTIF(Data!AN5:AW21,B25)</f>
+        <v>8</v>
+      </c>
+      <c r="D25" s="21">
+        <f t="shared" ref="D25:D27" si="3">C25/C$28*100</f>
+        <v>15.686274509803921</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <f>COUNTIF(Data!AN5:AW21,B26)</f>
+        <v>15</v>
+      </c>
+      <c r="D26" s="21">
+        <f t="shared" si="3"/>
+        <v>29.411764705882355</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27">
+        <f>COUNTIF(Data!AN5:AW21,B27)</f>
+        <v>24</v>
+      </c>
+      <c r="D27" s="21">
+        <f t="shared" si="3"/>
+        <v>47.058823529411761</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28">
+        <f>SUM(C24:C27)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B29" s="18"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B30" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31">
+        <f>COUNTIF(Data!AX5:BH21,B31)</f>
+        <v>3</v>
+      </c>
+      <c r="D31" s="21">
+        <f>C31/C$35*100</f>
+        <v>5.8823529411764701</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="20">
+        <f>COUNTIF(Data!AX5:BH21,B32) - 17</f>
+        <v>6</v>
+      </c>
+      <c r="D32" s="21">
+        <f t="shared" ref="D32:D34" si="4">C32/C$35*100</f>
+        <v>11.76470588235294</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33">
+        <f>COUNTIF(Data!AX5:BH21,B33)</f>
+        <v>22</v>
+      </c>
+      <c r="D33" s="21">
+        <f t="shared" si="4"/>
+        <v>43.137254901960787</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34">
+        <f>COUNTIF(Data!AX5:BH21,B34)</f>
+        <v>20</v>
+      </c>
+      <c r="D34" s="21">
+        <f t="shared" si="4"/>
+        <v>39.215686274509807</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B35" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35">
+        <f>SUM(C31:C34)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B36" s="18"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B37" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38">
+        <f>COUNTIF(Data!BI5:BR21,B38)</f>
+        <v>4</v>
+      </c>
+      <c r="D38" s="21">
+        <f>C38/C$42*100</f>
+        <v>7.8431372549019605</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39">
+        <f>COUNTIF(Data!BI5:BR21,B39)</f>
+        <v>10</v>
+      </c>
+      <c r="D39" s="21">
+        <f t="shared" ref="D39:D41" si="5">C39/C$42*100</f>
+        <v>19.607843137254903</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40">
+        <f>COUNTIF(Data!BI5:BR21,B40)</f>
+        <v>19</v>
+      </c>
+      <c r="D40" s="21">
+        <f t="shared" si="5"/>
+        <v>37.254901960784316</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41">
+        <f>COUNTIF(Data!BI5:BR21,B41)</f>
+        <v>18</v>
+      </c>
+      <c r="D41" s="21">
+        <f t="shared" si="5"/>
+        <v>35.294117647058826</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B42" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42">
+        <f>SUM(C38:C41)</f>
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>